<commit_message>
A few more context completion cases taken care of
</commit_message>
<xml_diff>
--- a/GeneroCompletionMap.xlsx
+++ b/GeneroCompletionMap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="339">
   <si>
     <t>Token just before cursor</t>
   </si>
@@ -1033,6 +1033,9 @@
   </si>
   <si>
     <t>then, (binary keywords)</t>
+  </si>
+  <si>
+    <t>to, like</t>
   </si>
 </sst>
 </file>
@@ -1454,11 +1457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C329"/>
+  <dimension ref="A1:C330"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B226" sqref="B226"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A291" sqref="A291:XFD291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4398,56 +4401,56 @@
         <v>242</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A291" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C291" s="5" t="s">
-        <v>170</v>
+    <row r="291" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B291" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C291" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B292" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C292" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B292" s="3" t="s">
+      <c r="B293" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A293" s="6" t="s">
+    <row r="294" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A294" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B293" s="7" t="s">
+      <c r="B294" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="C293" s="6" t="s">
+      <c r="C294" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A294" s="5" t="s">
+    <row r="295" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A295" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B294" s="3" t="s">
+      <c r="B295" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C294" s="5" t="s">
+      <c r="C295" s="5" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A295" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B295" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C295" s="6" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="296" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4455,10 +4458,10 @@
         <v>232</v>
       </c>
       <c r="B296" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C296" s="6" t="s">
-        <v>106</v>
+        <v>254</v>
       </c>
     </row>
     <row r="297" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4466,38 +4469,38 @@
         <v>232</v>
       </c>
       <c r="B297" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C297" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A298" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B298" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C297" s="6" t="s">
+      <c r="C298" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="298" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="6" t="s">
+    <row r="299" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B298" s="7" t="s">
+      <c r="B299" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="C298" s="6"/>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A299" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B299" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C299" s="5" t="s">
-        <v>169</v>
-      </c>
+      <c r="C299" s="6"/>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>188</v>
+        <v>102</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>169</v>
@@ -4505,43 +4508,43 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="5" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>28</v>
+        <v>188</v>
+      </c>
+      <c r="C301" s="5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B302" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B302" s="3" t="s">
+      <c r="B303" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C302" s="5" t="s">
+      <c r="C303" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A303" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B303" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C303" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A304" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C304" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -4549,91 +4552,91 @@
         <v>32</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>231</v>
+        <v>53</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C306" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B306" s="3" t="s">
+      <c r="B307" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C306" s="5" t="s">
+      <c r="C307" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="307" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A307" s="5" t="s">
+    <row r="308" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A308" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B307" s="3" t="s">
+      <c r="B308" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="308" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A308" s="6" t="s">
+    <row r="309" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="B308" s="7" t="s">
+      <c r="B309" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="C308" s="6" t="s">
+      <c r="C309" s="6" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A309" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B309" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B310" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B310" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A311" s="6" t="s">
+      <c r="B311" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B311" s="7" t="s">
+      <c r="B312" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C311" s="6" t="s">
+      <c r="C312" s="6" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B312" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="5" t="s">
-        <v>161</v>
+        <v>60</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B314" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C314" s="5" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -4641,89 +4644,89 @@
         <v>37</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C315" s="5" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="5" t="s">
-        <v>203</v>
+        <v>37</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="5" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>55</v>
+        <v>92</v>
+      </c>
+      <c r="C317" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B319" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B319" s="3" t="s">
+      <c r="B320" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C319" s="5" t="s">
+      <c r="C320" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="320" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A320" s="6" t="s">
+    <row r="321" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A321" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B320" s="7" t="s">
+      <c r="B321" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C320" s="6" t="s">
+      <c r="C321" s="6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" s="5" t="s">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B321" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A322" s="6" t="s">
+      <c r="B322" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A323" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B322" s="7" t="s">
+      <c r="B323" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C322" s="6" t="s">
+      <c r="C323" s="6" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B323" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C323" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -4731,10 +4734,10 @@
         <v>75</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="C324" s="5" t="s">
-        <v>181</v>
+        <v>68</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -4742,21 +4745,21 @@
         <v>75</v>
       </c>
       <c r="B325" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C325" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B326" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C325" s="5" t="s">
+      <c r="C326" s="5" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A326" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B326" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="C326" s="6" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="327" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4764,31 +4767,42 @@
         <v>75</v>
       </c>
       <c r="B327" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C327" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B328" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="C327" s="6" t="s">
+      <c r="C328" s="6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A328" s="5" t="s">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B328" s="3" t="s">
+      <c r="B329" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C328" s="5" t="s">
+      <c r="C329" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="329" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A329" s="6" t="s">
+    <row r="330" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A330" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B329" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C329" s="6" t="s">
+      <c r="B330" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C330" s="6" t="s">
         <v>226</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added missing backward search item for "=" context
</commit_message>
<xml_diff>
--- a/GeneroCompletionMap.xlsx
+++ b/GeneroCompletionMap.xlsx
@@ -393,9 +393,6 @@
     <t>as</t>
   </si>
   <si>
-    <t>let, for, if, where</t>
-  </si>
-  <si>
     <t>GreaterThan (&gt;)</t>
   </si>
   <si>
@@ -1039,6 +1036,9 @@
   </si>
   <si>
     <t>(from, prepare)</t>
+  </si>
+  <si>
+    <t>let, for, if, where, when</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1463,8 @@
   <dimension ref="A1:C332"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1493,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1523,10 +1523,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1578,7 +1578,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>99</v>
@@ -1589,7 +1589,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>102</v>
@@ -1614,7 +1614,7 @@
         <v>119</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1622,10 +1622,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>121</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
         <v>120</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1655,10 +1655,10 @@
         <v>25</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1666,7 +1666,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="6"/>
     </row>
@@ -1675,10 +1675,10 @@
         <v>25</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1686,10 +1686,10 @@
         <v>25</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1697,10 +1697,10 @@
         <v>25</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1708,10 +1708,10 @@
         <v>25</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -1719,10 +1719,10 @@
         <v>25</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1730,10 +1730,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -1741,10 +1741,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1752,10 +1752,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1763,10 +1763,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1774,10 +1774,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1785,10 +1785,10 @@
         <v>25</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1796,10 +1796,10 @@
         <v>25</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1807,10 +1807,10 @@
         <v>25</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1818,10 +1818,10 @@
         <v>25</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1829,10 +1829,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1840,10 +1840,10 @@
         <v>25</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1854,7 +1854,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1862,10 +1862,10 @@
         <v>25</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1873,10 +1873,10 @@
         <v>25</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1887,23 +1887,23 @@
         <v>28</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>55</v>
@@ -1912,10 +1912,10 @@
     </row>
     <row r="41" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>276</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>277</v>
       </c>
       <c r="C41" s="6"/>
     </row>
@@ -1932,10 +1932,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>55</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>3</v>
@@ -2003,7 +2003,7 @@
         <v>55</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2022,15 +2022,15 @@
         <v>123</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>55</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>55</v>
@@ -2046,38 +2046,38 @@
     </row>
     <row r="55" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C57" s="6"/>
     </row>
     <row r="58" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>55</v>
@@ -2086,46 +2086,46 @@
     </row>
     <row r="59" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -2141,7 +2141,7 @@
         <v>80</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>83</v>
@@ -2160,19 +2160,19 @@
     </row>
     <row r="66" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C66" s="6"/>
     </row>
     <row r="67" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C67" s="6"/>
     </row>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>55</v>
@@ -2203,7 +2203,7 @@
         <v>3</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -2214,7 +2214,7 @@
         <v>44</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2266,7 +2266,7 @@
         <v>55</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,24 +2274,24 @@
         <v>4</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>255</v>
       </c>
       <c r="C78" s="6"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>55</v>
@@ -2313,20 +2313,20 @@
         <v>28</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>70</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>30</v>
@@ -2345,24 +2345,24 @@
     </row>
     <row r="85" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B86" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>297</v>
-      </c>
       <c r="C86" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>32</v>
@@ -2394,18 +2394,18 @@
     </row>
     <row r="90" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>3</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>119</v>
@@ -2446,10 +2446,10 @@
     </row>
     <row r="96" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C96" s="6"/>
     </row>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>55</v>
@@ -2474,21 +2474,21 @@
     </row>
     <row r="99" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="B99" s="7" t="s">
-        <v>246</v>
-      </c>
       <c r="C99" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2501,7 +2501,7 @@
     </row>
     <row r="102" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>28</v>
@@ -2513,7 +2513,7 @@
         <v>38</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C103" s="6"/>
     </row>
@@ -2525,7 +2525,7 @@
         <v>55</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>124</v>
+        <v>339</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,12 +2536,12 @@
         <v>44</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>55</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>92</v>
@@ -2560,7 +2560,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>55</v>
@@ -2568,22 +2568,22 @@
     </row>
     <row r="109" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C109" s="6"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>55</v>
@@ -2604,10 +2604,10 @@
     </row>
     <row r="113" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B113" s="7" t="s">
         <v>307</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>308</v>
       </c>
       <c r="C113" s="6"/>
     </row>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="115" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B115" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="B115" s="11" t="s">
-        <v>278</v>
-      </c>
       <c r="C115" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,18 +2649,18 @@
         <v>112</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="118" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C118" s="6"/>
     </row>
@@ -2688,24 +2688,24 @@
         <v>88</v>
       </c>
       <c r="B121" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="122" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C122" s="6"/>
     </row>
     <row r="123" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>28</v>
@@ -2716,13 +2716,13 @@
     </row>
     <row r="124" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B124" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>32</v>
@@ -2749,13 +2749,13 @@
     </row>
     <row r="127" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B127" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2763,7 +2763,7 @@
         <v>59</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C128" s="6"/>
     </row>
@@ -2775,7 +2775,7 @@
         <v>52</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -2786,7 +2786,7 @@
         <v>55</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2797,7 +2797,7 @@
         <v>44</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>55</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>55</v>
@@ -2864,10 +2864,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>119</v>
@@ -2875,27 +2875,27 @@
     </row>
     <row r="140" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B141" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B141" s="7" t="s">
+      <c r="C141" s="6" t="s">
         <v>299</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B142" s="7" t="s">
         <v>32</v>
@@ -2906,18 +2906,18 @@
     </row>
     <row r="143" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B143" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="144" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>55</v>
@@ -2940,7 +2940,7 @@
         <v>42</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2948,10 +2948,10 @@
         <v>102</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2967,13 +2967,13 @@
     </row>
     <row r="149" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3003,7 +3003,7 @@
         <v>3</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="153" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3011,10 +3011,10 @@
         <v>57</v>
       </c>
       <c r="B153" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C153" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="C153" s="6" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="154" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3022,10 +3022,10 @@
         <v>57</v>
       </c>
       <c r="B154" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C154" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="C154" s="6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="155" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3033,21 +3033,21 @@
         <v>57</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3060,40 +3060,40 @@
     </row>
     <row r="158" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B158" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C158" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="159" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B159" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C159" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="C159" s="6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="160" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>108</v>
@@ -3101,10 +3101,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -3123,7 +3123,7 @@
         <v>44</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>3</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -3147,7 +3147,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -3171,13 +3171,13 @@
     </row>
     <row r="170" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="171" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3208,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -3219,7 +3219,7 @@
         <v>55</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>44</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -3258,10 +3258,10 @@
         <v>35</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -3269,15 +3269,15 @@
         <v>35</v>
       </c>
       <c r="B179" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C179" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="C179" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>55</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>55</v>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="186" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B186" s="7" t="s">
         <v>119</v>
@@ -3348,10 +3348,10 @@
     </row>
     <row r="188" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="C188" s="5" t="s">
         <v>75</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>55</v>
@@ -3375,18 +3375,18 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>55</v>
@@ -3394,10 +3394,10 @@
     </row>
     <row r="193" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C193" s="6"/>
     </row>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="195" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B195" s="7" t="s">
         <v>55</v>
@@ -3423,7 +3423,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>32</v>
@@ -3434,29 +3434,29 @@
     </row>
     <row r="197" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B197" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>55</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>32</v>
@@ -3475,52 +3475,52 @@
     </row>
     <row r="201" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B201" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C201" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="202" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C202" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="B202" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C202" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="203" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B203" s="7" t="s">
         <v>256</v>
-      </c>
-      <c r="B203" s="7" t="s">
-        <v>257</v>
       </c>
       <c r="C203" s="6"/>
     </row>
     <row r="204" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>75</v>
@@ -3542,7 +3542,7 @@
         <v>42</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C207" s="5"/>
     </row>
@@ -3562,10 +3562,10 @@
         <v>42</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="210" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3573,7 +3573,7 @@
         <v>42</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C210" s="6" t="s">
         <v>120</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="211" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>55</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="212" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>55</v>
@@ -3624,10 +3624,10 @@
         <v>36</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="216" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -3635,10 +3635,10 @@
         <v>36</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C216" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="217" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3649,7 +3649,7 @@
         <v>32</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="218" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3657,7 +3657,7 @@
         <v>36</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>99</v>
@@ -3679,7 +3679,7 @@
         <v>36</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>102</v>
@@ -3690,7 +3690,7 @@
         <v>36</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C221" s="6"/>
     </row>
@@ -3699,10 +3699,10 @@
         <v>36</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C222" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -3721,27 +3721,27 @@
         <v>70</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="225" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B225" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="B225" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="C225" s="6"/>
     </row>
     <row r="226" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C226" s="6"/>
     </row>
@@ -3755,29 +3755,29 @@
     </row>
     <row r="228" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B228" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="229" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B229" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C229" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="C229" s="6" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>55</v>
@@ -3785,7 +3785,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>3</v>
@@ -3796,10 +3796,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C232" s="5" t="s">
         <v>119</v>
@@ -3807,40 +3807,40 @@
     </row>
     <row r="233" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B233" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C233" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="C233" s="6" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="234" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B234" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C234" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="C234" s="6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="235" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C235" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>55</v>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="237" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B237" s="7" t="s">
         <v>3</v>
@@ -3857,35 +3857,35 @@
     </row>
     <row r="238" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C238" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B239" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B239" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="C239" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="240" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C240" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -3898,10 +3898,10 @@
     </row>
     <row r="242" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B242" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C242" s="6"/>
     </row>
@@ -3929,24 +3929,24 @@
     </row>
     <row r="245" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B245" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="246" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B246" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C246" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="247" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -3954,10 +3954,10 @@
         <v>8</v>
       </c>
       <c r="B247" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C247" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -3973,7 +3973,7 @@
     </row>
     <row r="249" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>75</v>
@@ -3985,13 +3985,13 @@
         <v>84</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C250" s="6"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>44</v>
@@ -4002,7 +4002,7 @@
         <v>100</v>
       </c>
       <c r="B252" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C252" s="6" t="s">
         <v>99</v>
@@ -4024,10 +4024,10 @@
         <v>100</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="255" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -4035,10 +4035,10 @@
         <v>100</v>
       </c>
       <c r="B255" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C255" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="256" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4057,7 +4057,7 @@
         <v>100</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -4065,10 +4065,10 @@
         <v>34</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C258" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="259" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -4076,10 +4076,10 @@
         <v>34</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C259" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -4142,7 +4142,7 @@
         <v>34</v>
       </c>
       <c r="B265" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C265" s="6" t="s">
         <v>99</v>
@@ -4175,7 +4175,7 @@
         <v>34</v>
       </c>
       <c r="B268" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C268" s="6" t="s">
         <v>120</v>
@@ -4186,7 +4186,7 @@
         <v>34</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -4194,10 +4194,10 @@
         <v>34</v>
       </c>
       <c r="B270" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C270" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="C270" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -4208,7 +4208,7 @@
         <v>3</v>
       </c>
       <c r="C271" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -4216,10 +4216,10 @@
         <v>34</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -4232,29 +4232,29 @@
     </row>
     <row r="274" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B274" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C274" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="275" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B275" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C275" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="276" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B276" s="7" t="s">
         <v>55</v>
@@ -4263,7 +4263,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B277" s="3" t="s">
         <v>32</v>
@@ -4274,13 +4274,13 @@
     </row>
     <row r="278" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B278" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C278" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -4293,35 +4293,35 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B281" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C281" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -4337,10 +4337,10 @@
     </row>
     <row r="284" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B284" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C284" s="6"/>
     </row>
@@ -4365,7 +4365,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B287" s="3" t="s">
         <v>92</v>
@@ -4393,7 +4393,7 @@
         <v>28</v>
       </c>
       <c r="C289" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -4409,10 +4409,10 @@
         <v>118</v>
       </c>
       <c r="B291" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C291" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="292" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4420,7 +4420,7 @@
         <v>118</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C292" s="6" t="s">
         <v>53</v>
@@ -4428,13 +4428,13 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B293" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -4447,43 +4447,43 @@
     </row>
     <row r="295" spans="1:3" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B295" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C295" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="296" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B296" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B296" s="3" t="s">
-        <v>233</v>
-      </c>
       <c r="C296" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="297" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C297" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="298" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B298" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C298" s="6" t="s">
         <v>106</v>
@@ -4491,55 +4491,55 @@
     </row>
     <row r="299" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B299" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C299" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="300" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B300" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="301" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B301" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="B301" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="C301" s="6"/>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B302" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B303" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B303" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="C303" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -4569,7 +4569,7 @@
         <v>30</v>
       </c>
       <c r="C306" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -4591,7 +4591,7 @@
         <v>55</v>
       </c>
       <c r="C308" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
     </row>
     <row r="310" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B310" s="3" t="s">
         <v>30</v>
@@ -4615,18 +4615,18 @@
     </row>
     <row r="311" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B311" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C311" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B312" s="3" t="s">
         <v>52</v>
@@ -4634,7 +4634,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B313" s="3" t="s">
         <v>55</v>
@@ -4642,13 +4642,13 @@
     </row>
     <row r="314" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B314" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C314" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -4661,7 +4661,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -4688,7 +4688,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B319" s="3" t="s">
         <v>92</v>
@@ -4721,7 +4721,7 @@
         <v>3</v>
       </c>
       <c r="C322" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="323" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4729,10 +4729,10 @@
         <v>120</v>
       </c>
       <c r="B323" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C323" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -4773,7 +4773,7 @@
         <v>3</v>
       </c>
       <c r="C327" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -4781,10 +4781,10 @@
         <v>75</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C328" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="329" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4792,10 +4792,10 @@
         <v>75</v>
       </c>
       <c r="B329" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C329" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="330" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4803,15 +4803,15 @@
         <v>75</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C330" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B331" s="3" t="s">
         <v>32</v>
@@ -4822,13 +4822,13 @@
     </row>
     <row r="332" spans="1:3" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A332" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B332" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C332" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>